<commit_message>
se elige la escala y se ajustan melodias
</commit_message>
<xml_diff>
--- a/Harmonizer/datasets/chords.xlsx
+++ b/Harmonizer/datasets/chords.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG33"/>
+  <dimension ref="A1:AK37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,127 +471,147 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>2_-</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>2_7</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>b3_</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>b3_-</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>b3_7</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>b3_º7</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>3_-</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>3_7</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>4_</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>4_-</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>4_7</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>b5_-b5</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>b5_º7</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>5_</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>5_-</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>5_-b5</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>5_7</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>5_º7</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>b6_</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>b6_-b5</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>b6_7</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>6_-</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>6_-b5</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>6_7</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>b7_</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>b7_-</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>b7_7</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>b7_º7</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>7_-b5</t>
         </is>
       </c>
     </row>
@@ -602,13 +622,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -629,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -647,22 +667,22 @@
         <v>0</v>
       </c>
       <c r="Q2" t="n">
+        <v>4</v>
+      </c>
+      <c r="R2" t="n">
         <v>2</v>
       </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
       <c r="S2" t="n">
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2" t="n">
         <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W2" t="n">
         <v>0</v>
@@ -671,14 +691,14 @@
         <v>0</v>
       </c>
       <c r="Y2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
         <v>2</v>
       </c>
-      <c r="Z2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
       <c r="AB2" t="n">
         <v>0</v>
       </c>
@@ -686,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="AD2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE2" t="n">
         <v>0</v>
@@ -695,6 +715,18 @@
         <v>0</v>
       </c>
       <c r="AG2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -705,7 +737,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -726,11 +758,11 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
         <v>2</v>
       </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
@@ -747,50 +779,50 @@
         <v>0</v>
       </c>
       <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>48</v>
       </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
       <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
         <v>4</v>
       </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
       <c r="T3" t="n">
         <v>0</v>
       </c>
       <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>7</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="n">
         <v>6</v>
       </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" t="n">
-        <v>0</v>
-      </c>
-      <c r="X3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>0</v>
-      </c>
       <c r="AE3" t="n">
         <v>0</v>
       </c>
@@ -798,6 +830,18 @@
         <v>0</v>
       </c>
       <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -835,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -850,11 +894,11 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
       <c r="R4" t="n">
         <v>0</v>
       </c>
@@ -871,7 +915,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -901,6 +945,18 @@
         <v>0</v>
       </c>
       <c r="AG4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1006,6 +1062,18 @@
       <c r="AG5" t="n">
         <v>0</v>
       </c>
+      <c r="AH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1056,11 +1124,11 @@
         <v>0</v>
       </c>
       <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
         <v>4</v>
       </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
       <c r="R6" t="n">
         <v>0</v>
       </c>
@@ -1101,12 +1169,24 @@
         <v>0</v>
       </c>
       <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="n">
         <v>4</v>
       </c>
-      <c r="AF6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG6" t="n">
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1168,14 +1248,14 @@
         <v>0</v>
       </c>
       <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
         <v>2</v>
       </c>
-      <c r="T7" t="n">
+      <c r="U7" t="n">
         <v>4</v>
       </c>
-      <c r="U7" t="n">
-        <v>0</v>
-      </c>
       <c r="V7" t="n">
         <v>0</v>
       </c>
@@ -1210,6 +1290,18 @@
         <v>0</v>
       </c>
       <c r="AG7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1250,11 +1342,11 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
         <v>8</v>
       </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
       <c r="N8" t="n">
         <v>0</v>
       </c>
@@ -1265,11 +1357,11 @@
         <v>0</v>
       </c>
       <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
         <v>8</v>
       </c>
-      <c r="R8" t="n">
-        <v>0</v>
-      </c>
       <c r="S8" t="n">
         <v>0</v>
       </c>
@@ -1280,14 +1372,14 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
         <v>4</v>
       </c>
-      <c r="W8" t="n">
-        <v>0</v>
-      </c>
-      <c r="X8" t="n">
-        <v>0</v>
-      </c>
       <c r="Y8" t="n">
         <v>0</v>
       </c>
@@ -1304,32 +1396,44 @@
         <v>0</v>
       </c>
       <c r="AD8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG8" t="n">
         <v>4</v>
       </c>
-      <c r="AE8" t="n">
+      <c r="AH8" t="n">
         <v>4</v>
       </c>
-      <c r="AF8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG8" t="n">
+      <c r="AI8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>2_7</t>
+          <t>2_-</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1416,23 +1520,35 @@
         <v>0</v>
       </c>
       <c r="AG9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>b3_</t>
+          <t>2_7</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1456,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -1471,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
@@ -1516,20 +1632,32 @@
         <v>0</v>
       </c>
       <c r="AF10" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>b3_-</t>
+          <t>b3_</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -1562,114 +1690,126 @@
         <v>0</v>
       </c>
       <c r="M11" t="n">
+        <v>2</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>8</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI11" t="n">
         <v>4</v>
       </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S11" t="n">
-        <v>0</v>
-      </c>
-      <c r="T11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U11" t="n">
-        <v>0</v>
-      </c>
-      <c r="V11" t="n">
-        <v>0</v>
-      </c>
-      <c r="W11" t="n">
-        <v>0</v>
-      </c>
-      <c r="X11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG11" t="n">
+      <c r="AJ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>b3_7</t>
+          <t>b3_-</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>0</v>
       </c>
       <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
         <v>4</v>
       </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>4</v>
-      </c>
-      <c r="H12" t="n">
-        <v>4</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>4</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
@@ -1701,13 +1841,13 @@
         <v>0</v>
       </c>
       <c r="Y12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Z12" t="n">
         <v>0</v>
       </c>
       <c r="AA12" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AB12" t="n">
         <v>0</v>
@@ -1725,20 +1865,32 @@
         <v>0</v>
       </c>
       <c r="AG12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>b3_º7</t>
+          <t>b3_7</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -1750,10 +1902,10 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -1762,17 +1914,17 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
         <v>4</v>
       </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
       <c r="O13" t="n">
         <v>0</v>
       </c>
@@ -1783,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
@@ -1810,13 +1962,13 @@
         <v>0</v>
       </c>
       <c r="AA13" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AB13" t="n">
         <v>0</v>
       </c>
       <c r="AC13" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD13" t="n">
         <v>0</v>
@@ -1828,20 +1980,32 @@
         <v>0</v>
       </c>
       <c r="AG13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>3_-</t>
+          <t>b3_º7</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -1868,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
@@ -1889,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="S14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T14" t="n">
         <v>0</v>
@@ -1931,13 +2095,25 @@
         <v>0</v>
       </c>
       <c r="AG14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>3_7</t>
+          <t>3_-</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -2013,13 +2189,13 @@
         <v>0</v>
       </c>
       <c r="Z15" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA15" t="n">
         <v>0</v>
       </c>
       <c r="AB15" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC15" t="n">
         <v>0</v>
@@ -2034,21 +2210,33 @@
         <v>0</v>
       </c>
       <c r="AG15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>4_</t>
+          <t>3_7</t>
         </is>
       </c>
       <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
         <v>2</v>
       </c>
-      <c r="C16" t="n">
-        <v>46</v>
-      </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
@@ -2056,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -2080,55 +2268,55 @@
         <v>0</v>
       </c>
       <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" t="n">
         <v>2</v>
       </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0</v>
-      </c>
-      <c r="T16" t="n">
-        <v>0</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0</v>
-      </c>
-      <c r="V16" t="n">
-        <v>0</v>
-      </c>
-      <c r="W16" t="n">
-        <v>4</v>
-      </c>
-      <c r="X16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>0</v>
-      </c>
       <c r="AC16" t="n">
         <v>0</v>
       </c>
       <c r="AD16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE16" t="n">
         <v>0</v>
@@ -2137,35 +2325,47 @@
         <v>0</v>
       </c>
       <c r="AG16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>4_-</t>
+          <t>4_</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C17" t="n">
+        <v>46</v>
+      </c>
+      <c r="D17" t="n">
         <v>2</v>
       </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -2177,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M17" t="n">
         <v>0</v>
@@ -2186,7 +2386,7 @@
         <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
@@ -2210,13 +2410,13 @@
         <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="X17" t="n">
         <v>0</v>
       </c>
       <c r="Y17" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Z17" t="n">
         <v>0</v>
@@ -2234,26 +2434,38 @@
         <v>0</v>
       </c>
       <c r="AE17" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AF17" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AG17" t="n">
         <v>0</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>4_7</t>
+          <t>4_-</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -2283,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N18" t="n">
         <v>0</v>
@@ -2337,26 +2549,38 @@
         <v>0</v>
       </c>
       <c r="AE18" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AF18" t="n">
         <v>0</v>
       </c>
       <c r="AG18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>12</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>b5_-b5</t>
+          <t>4_7</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -2371,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -2446,20 +2670,32 @@
         <v>0</v>
       </c>
       <c r="AG19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>8</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>b5_º7</t>
+          <t>b5_-b5</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -2504,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="R20" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
@@ -2516,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="V20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" t="n">
         <v>0</v>
@@ -2549,13 +2785,25 @@
         <v>0</v>
       </c>
       <c r="AG20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>5_</t>
+          <t>b5_º7</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -2598,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P21" t="n">
         <v>0</v>
@@ -2610,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="S21" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T21" t="n">
         <v>0</v>
@@ -2652,20 +2900,32 @@
         <v>0</v>
       </c>
       <c r="AG21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK21" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>5_-b5</t>
+          <t>5_</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -2692,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M22" t="n">
         <v>0</v>
@@ -2704,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="P22" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q22" t="n">
         <v>0</v>
@@ -2716,7 +2976,7 @@
         <v>0</v>
       </c>
       <c r="T22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22" t="n">
         <v>0</v>
@@ -2755,20 +3015,32 @@
         <v>0</v>
       </c>
       <c r="AG22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>5_7</t>
+          <t>5_-</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -2786,13 +3058,13 @@
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" t="n">
         <v>0</v>
@@ -2810,7 +3082,7 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23" t="n">
         <v>0</v>
@@ -2846,25 +3118,37 @@
         <v>0</v>
       </c>
       <c r="AC23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG23" t="n">
         <v>6</v>
       </c>
-      <c r="AD23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG23" t="n">
+      <c r="AH23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK23" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>5_º7</t>
+          <t>5_-b5</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -2901,7 +3185,7 @@
         <v>0</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
@@ -2955,26 +3239,38 @@
         <v>0</v>
       </c>
       <c r="AE24" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AF24" t="n">
         <v>0</v>
       </c>
       <c r="AG24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>b6_</t>
+          <t>5_7</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -2995,13 +3291,13 @@
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K25" t="n">
         <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
         <v>0</v>
@@ -3016,7 +3312,7 @@
         <v>0</v>
       </c>
       <c r="Q25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R25" t="n">
         <v>0</v>
@@ -3031,7 +3327,7 @@
         <v>0</v>
       </c>
       <c r="V25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W25" t="n">
         <v>0</v>
@@ -3061,16 +3357,28 @@
         <v>0</v>
       </c>
       <c r="AF25" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AG25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK25" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>b6_-b5</t>
+          <t>5_º7</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -3152,7 +3460,7 @@
         <v>0</v>
       </c>
       <c r="AB26" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC26" t="n">
         <v>0</v>
@@ -3167,17 +3475,29 @@
         <v>0</v>
       </c>
       <c r="AG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK26" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>b6_7</t>
+          <t>b6_</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -3186,47 +3506,47 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
         <v>4</v>
       </c>
-      <c r="F27" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" t="n">
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>2</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
         <v>4</v>
       </c>
-      <c r="I27" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q27" t="n">
-        <v>0</v>
-      </c>
-      <c r="R27" t="n">
-        <v>0</v>
-      </c>
       <c r="S27" t="n">
         <v>0</v>
       </c>
@@ -3270,102 +3590,114 @@
         <v>0</v>
       </c>
       <c r="AG27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>6_-</t>
+          <t>b6_-b5</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>0</v>
       </c>
       <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD28" t="n">
         <v>2</v>
       </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>2</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" t="n">
-        <v>2</v>
-      </c>
-      <c r="J28" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" t="n">
-        <v>0</v>
-      </c>
-      <c r="O28" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R28" t="n">
-        <v>0</v>
-      </c>
-      <c r="S28" t="n">
-        <v>0</v>
-      </c>
-      <c r="T28" t="n">
-        <v>0</v>
-      </c>
-      <c r="U28" t="n">
-        <v>0</v>
-      </c>
-      <c r="V28" t="n">
-        <v>0</v>
-      </c>
-      <c r="W28" t="n">
-        <v>6</v>
-      </c>
-      <c r="X28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD28" t="n">
-        <v>0</v>
-      </c>
       <c r="AE28" t="n">
         <v>0</v>
       </c>
@@ -3373,13 +3705,25 @@
         <v>0</v>
       </c>
       <c r="AG28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK28" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>6_7</t>
+          <t>b6_7</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -3392,7 +3736,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -3401,7 +3745,7 @@
         <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
@@ -3461,7 +3805,7 @@
         <v>0</v>
       </c>
       <c r="AB29" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AC29" t="n">
         <v>0</v>
@@ -3476,20 +3820,32 @@
         <v>0</v>
       </c>
       <c r="AG29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK29" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>b7_</t>
+          <t>6_-</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -3501,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -3510,29 +3866,29 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K30" t="n">
         <v>0</v>
       </c>
       <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
         <v>4</v>
       </c>
-      <c r="M30" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q30" t="n">
-        <v>0</v>
-      </c>
       <c r="R30" t="n">
         <v>0</v>
       </c>
@@ -3555,7 +3911,7 @@
         <v>0</v>
       </c>
       <c r="Y30" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Z30" t="n">
         <v>0</v>
@@ -3579,13 +3935,25 @@
         <v>0</v>
       </c>
       <c r="AG30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK30" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>b7_-</t>
+          <t>6_-b5</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -3601,13 +3969,13 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
@@ -3619,7 +3987,7 @@
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M31" t="n">
         <v>0</v>
@@ -3634,7 +4002,7 @@
         <v>0</v>
       </c>
       <c r="Q31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R31" t="n">
         <v>0</v>
@@ -3655,7 +4023,7 @@
         <v>0</v>
       </c>
       <c r="X31" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Y31" t="n">
         <v>0</v>
@@ -3682,13 +4050,25 @@
         <v>0</v>
       </c>
       <c r="AG31" t="n">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>b7_7</t>
+          <t>6_7</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -3716,68 +4096,68 @@
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K32" t="n">
         <v>0</v>
       </c>
       <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD32" t="n">
         <v>6</v>
       </c>
-      <c r="M32" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" t="n">
-        <v>0</v>
-      </c>
-      <c r="O32" t="n">
-        <v>0</v>
-      </c>
-      <c r="P32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>0</v>
-      </c>
-      <c r="R32" t="n">
-        <v>0</v>
-      </c>
-      <c r="S32" t="n">
-        <v>0</v>
-      </c>
-      <c r="T32" t="n">
-        <v>0</v>
-      </c>
-      <c r="U32" t="n">
-        <v>0</v>
-      </c>
-      <c r="V32" t="n">
-        <v>0</v>
-      </c>
-      <c r="W32" t="n">
-        <v>0</v>
-      </c>
-      <c r="X32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD32" t="n">
-        <v>0</v>
-      </c>
       <c r="AE32" t="n">
         <v>0</v>
       </c>
@@ -3785,109 +4165,593 @@
         <v>0</v>
       </c>
       <c r="AG32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
+          <t>b7_</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>6</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>4</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>6</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>b7_-</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>4</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>8</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>4</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>b7_7</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>10</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>6</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
           <t>b7_º7</t>
         </is>
       </c>
-      <c r="B33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" t="n">
-        <v>0</v>
-      </c>
-      <c r="O33" t="n">
-        <v>0</v>
-      </c>
-      <c r="P33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q33" t="n">
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="n">
         <v>4</v>
       </c>
-      <c r="R33" t="n">
-        <v>0</v>
-      </c>
-      <c r="S33" t="n">
-        <v>0</v>
-      </c>
-      <c r="T33" t="n">
-        <v>0</v>
-      </c>
-      <c r="U33" t="n">
-        <v>0</v>
-      </c>
-      <c r="V33" t="n">
-        <v>0</v>
-      </c>
-      <c r="W33" t="n">
-        <v>0</v>
-      </c>
-      <c r="X33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG33" t="n">
+      <c r="S36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0</v>
+      </c>
+      <c r="V36" t="n">
+        <v>0</v>
+      </c>
+      <c r="W36" t="n">
+        <v>0</v>
+      </c>
+      <c r="X36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>7_-b5</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W37" t="n">
+        <v>0</v>
+      </c>
+      <c r="X37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK37" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modos arreglados y terminados
</commit_message>
<xml_diff>
--- a/Harmonizer/datasets/chords.xlsx
+++ b/Harmonizer/datasets/chords.xlsx
@@ -683,7 +683,7 @@
         <v>73</v>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1006,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -1054,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="AC4" t="n">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="AD4" t="n">
         <v>0</v>
@@ -1861,7 +1861,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -1954,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="AG10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10" t="n">
         <v>0</v>
@@ -2311,7 +2311,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -2329,7 +2329,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -4679,7 +4679,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -4793,7 +4793,7 @@
         <v>0</v>
       </c>
       <c r="AP29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AQ29" t="n">
         <v>0</v>
@@ -5289,7 +5289,7 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" t="n">
         <v>0</v>
@@ -6678,7 +6678,7 @@
         <v>0</v>
       </c>
       <c r="AC42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD42" t="n">
         <v>0</v>

</xml_diff>